<commit_message>
Exemplo de uso da ferramenta
</commit_message>
<xml_diff>
--- a/trabalho CMMI1.xlsx
+++ b/trabalho CMMI1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ambro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenne\Documents\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C26E352-FE71-4FBB-B2B7-AC80E4BFE6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53561C7-C01D-4BAC-9A81-8FBA1CEA9449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -654,19 +654,20 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="177.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="177.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -700,7 +701,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -711,7 +712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -722,7 +723,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -733,7 +734,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -744,7 +745,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -755,7 +756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
@@ -768,7 +769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -779,7 +780,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -790,7 +791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -801,7 +802,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -812,7 +813,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -823,7 +824,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -834,7 +835,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -845,7 +846,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -856,7 +857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13" t="s">
@@ -869,7 +870,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -880,7 +881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -891,7 +892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -902,119 +903,119 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="16.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>

</xml_diff>